<commit_message>
- ADD Promises to be able to run categorize() after reading Excel file
</commit_message>
<xml_diff>
--- a/keywords.xlsx
+++ b/keywords.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>aldi</t>
   </si>
@@ -28,6 +28,18 @@
   </si>
   <si>
     <t>Restaurant</t>
+  </si>
+  <si>
+    <t>Some spaces</t>
+  </si>
+  <si>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>Income</t>
+  </si>
+  <si>
+    <t>$tr@ng€ Нейм</t>
   </si>
 </sst>
 </file>
@@ -366,10 +378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -394,8 +406,25 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
- FIX processing of keywords and saving results back to CSV
</commit_message>
<xml_diff>
--- a/keywords.xlsx
+++ b/keywords.xlsx
@@ -16,30 +16,231 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>aldi</t>
-  </si>
-  <si>
-    <t>Food</t>
-  </si>
-  <si>
-    <t>McDonalds</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="75">
   <si>
     <t>Restaurant</t>
   </si>
   <si>
-    <t>Some spaces</t>
-  </si>
-  <si>
-    <t>Default</t>
-  </si>
-  <si>
     <t>Income</t>
   </si>
   <si>
-    <t>$tr@ng€ Нейм</t>
+    <t>1u1</t>
+  </si>
+  <si>
+    <t>Internet</t>
+  </si>
+  <si>
+    <t>ALDI</t>
+  </si>
+  <si>
+    <t>Lebensmittel</t>
+  </si>
+  <si>
+    <t>Aldi Talk</t>
+  </si>
+  <si>
+    <t>Handy</t>
+  </si>
+  <si>
+    <t>AMAZON</t>
+  </si>
+  <si>
+    <t>Einkauf</t>
+  </si>
+  <si>
+    <t>ARAL</t>
+  </si>
+  <si>
+    <t>Auto</t>
+  </si>
+  <si>
+    <t>AUTOHAUS NIX</t>
+  </si>
+  <si>
+    <t>BUERGERAMT</t>
+  </si>
+  <si>
+    <t>C+A</t>
+  </si>
+  <si>
+    <t>Kleidung</t>
+  </si>
+  <si>
+    <t>CINESTAR</t>
+  </si>
+  <si>
+    <t>Hobby/Entertainment</t>
+  </si>
+  <si>
+    <t>DECATHLON</t>
+  </si>
+  <si>
+    <t>DEICHMANN</t>
+  </si>
+  <si>
+    <t>DEUTSCHE POST</t>
+  </si>
+  <si>
+    <t>Post</t>
+  </si>
+  <si>
+    <t>DM</t>
+  </si>
+  <si>
+    <t>Drogerie</t>
+  </si>
+  <si>
+    <t>EBAY</t>
+  </si>
+  <si>
+    <t>Familienkasse</t>
+  </si>
+  <si>
+    <t>GAA</t>
+  </si>
+  <si>
+    <t>Cash</t>
+  </si>
+  <si>
+    <t>IKEA</t>
+  </si>
+  <si>
+    <t>Moebel</t>
+  </si>
+  <si>
+    <t>ING-DiBa</t>
+  </si>
+  <si>
+    <t>Darlehen</t>
+  </si>
+  <si>
+    <t>INTERTOYS</t>
+  </si>
+  <si>
+    <t>Kinder</t>
+  </si>
+  <si>
+    <t>Kartenumsatz</t>
+  </si>
+  <si>
+    <t>Kreditkarte</t>
+  </si>
+  <si>
+    <t>MADE BY YOU</t>
+  </si>
+  <si>
+    <t>Mainova</t>
+  </si>
+  <si>
+    <t>Nebenkosten</t>
+  </si>
+  <si>
+    <t>MCDONALDS</t>
+  </si>
+  <si>
+    <t>Musikschule</t>
+  </si>
+  <si>
+    <t>NANU-NANA</t>
+  </si>
+  <si>
+    <t>NETTO</t>
+  </si>
+  <si>
+    <t>NINTENDO</t>
+  </si>
+  <si>
+    <t>OLES PIDGORNYY</t>
+  </si>
+  <si>
+    <t>Ordnungsamt</t>
+  </si>
+  <si>
+    <t>PayPal</t>
+  </si>
+  <si>
+    <t>Penny</t>
+  </si>
+  <si>
+    <t>REAL</t>
+  </si>
+  <si>
+    <t>REWE</t>
+  </si>
+  <si>
+    <t>ROSSMANN</t>
+  </si>
+  <si>
+    <t>Samariter</t>
+  </si>
+  <si>
+    <t>Schwimmclub</t>
+  </si>
+  <si>
+    <t>Shell</t>
+  </si>
+  <si>
+    <t>SIMON + STOLLE</t>
+  </si>
+  <si>
+    <t>Sparen</t>
+  </si>
+  <si>
+    <t>SPORTARENA</t>
+  </si>
+  <si>
+    <t>STADLER</t>
+  </si>
+  <si>
+    <t>Transport</t>
+  </si>
+  <si>
+    <t>Stadtentwaesserung</t>
+  </si>
+  <si>
+    <t>TARGOBANK</t>
+  </si>
+  <si>
+    <t>Tchibo</t>
+  </si>
+  <si>
+    <t>Techniker Krankenkasse</t>
+  </si>
+  <si>
+    <t>Krankengeld</t>
+  </si>
+  <si>
+    <t>tegut</t>
+  </si>
+  <si>
+    <t>Telekom</t>
+  </si>
+  <si>
+    <t>Telefon</t>
+  </si>
+  <si>
+    <t>Tickets</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>UNIVERSITAET</t>
+  </si>
+  <si>
+    <t>Education</t>
+  </si>
+  <si>
+    <t>VGF</t>
+  </si>
+  <si>
+    <t>Volkshochschule</t>
+  </si>
+  <si>
+    <t>WOOLWORTH</t>
+  </si>
+  <si>
+    <t>ZEEMAN</t>
   </si>
 </sst>
 </file>
@@ -378,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -392,34 +593,434 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>49</v>
+      </c>
+      <c r="B33" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>50</v>
+      </c>
+      <c r="B34" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>51</v>
+      </c>
+      <c r="B35" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>52</v>
+      </c>
+      <c r="B36" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>53</v>
+      </c>
+      <c r="B37" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>54</v>
+      </c>
+      <c r="B38" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>55</v>
+      </c>
+      <c r="B39" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>56</v>
+      </c>
+      <c r="B40" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>57</v>
+      </c>
+      <c r="B41" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>59</v>
+      </c>
+      <c r="B42" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>60</v>
+      </c>
+      <c r="B43" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>61</v>
+      </c>
+      <c r="B44" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>62</v>
+      </c>
+      <c r="B45" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>64</v>
+      </c>
+      <c r="B46" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>65</v>
+      </c>
+      <c r="B47" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>67</v>
+      </c>
+      <c r="B48" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>68</v>
+      </c>
+      <c r="B49" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>69</v>
+      </c>
+      <c r="B50" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>71</v>
+      </c>
+      <c r="B51" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>72</v>
+      </c>
+      <c r="B52" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>73</v>
+      </c>
+      <c r="B53" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>74</v>
+      </c>
+      <c r="B54" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>